<commit_message>
Dataframe and Search Engine
Foi atualizada a mecanica de busca para que buscasse através da tabela do excell os parametros. E foi criado o dataframe com o resultado final, apresentando Produto, Preço, Link e Fonte de busca.
Atualizado a planilha de busca no elemento preço máximo, para que aparecesse mais resultados na busca, ao invés de resultado em branco.
</commit_message>
<xml_diff>
--- a/buscas.xlsx
+++ b/buscas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magal\OneDrive\Área de Trabalho\aula python\Projeto 02 Automação Web\Automacao-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2313C8-AEED-4198-A70C-BD89DEEA04C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF59E00-B133-4812-9529-FE7D55F95BEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4110" yWindow="3345" windowWidth="18900" windowHeight="11055" xr2:uid="{CD3F9E8B-8E7C-43BA-8194-A874F6873E6D}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
         <v>3000</v>
       </c>
       <c r="D2">
-        <v>3500</v>
+        <v>4900</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>